<commit_message>
added linux postinstall, fixed floating points, fixed default data, added classic save features
</commit_message>
<xml_diff>
--- a/template_sekundarstufe_1.xlsx
+++ b/template_sekundarstufe_1.xlsx
@@ -11,6 +11,8 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tasks" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grades" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Additional" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Points" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Score" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -69,6 +71,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -572,17 +642,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3 (9.7%)</t>
+          <t>6 (19.4%)</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" t="n">
         <v>3</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -1170,4 +1240,315 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Points</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Grade</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Students</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Student E</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>5-</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Student D</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>4-</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Student G</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>3-</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Student C</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Student H</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>3+</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Student I</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2-</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Student A, Student J</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1-</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Student B, Student F</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Grade</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Amount</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Students</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Student B, Student F</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Student A, Student J</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Student C, Student H, Student I</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Student G</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Student D</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Student E</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
autosaving working - issues when autosave is disabled
</commit_message>
<xml_diff>
--- a/template_sekundarstufe_1.xlsx
+++ b/template_sekundarstufe_1.xlsx
@@ -494,7 +494,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2-</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -502,7 +502,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>22 (71.0%)</t>
+          <t>23.0 (74.2%)</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -512,7 +512,7 @@
         <v>8</v>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2" t="n">
         <v>6</v>
@@ -537,7 +537,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>27 (87.1%)</t>
+          <t>27.0 (87.1%)</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -572,7 +572,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>17 (54.8%)</t>
+          <t>18.0 (58.1%)</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -582,7 +582,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H4" t="n">
         <v>6</v>
@@ -607,7 +607,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>9 (29.0%)</t>
+          <t>9.0 (29.0%)</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -642,7 +642,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>6 (19.4%)</t>
+          <t>6.0 (19.4%)</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -677,7 +677,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>27 (87.1%)</t>
+          <t>27.0 (87.1%)</t>
         </is>
       </c>
       <c r="E7" t="n">
@@ -712,7 +712,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>13 (41.9%)</t>
+          <t>13.0 (41.9%)</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -747,7 +747,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>19 (61.3%)</t>
+          <t>19.0 (61.3%)</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -782,7 +782,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>20 (64.5%)</t>
+          <t>20.0 (64.5%)</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -817,7 +817,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>22 (71.0%)</t>
+          <t>22.0 (71.0%)</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -1248,7 +1248,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1334,7 +1334,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1396,27 +1396,45 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Student A, Student J</t>
+          <t>Student J</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Student A</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B10" t="inlineStr">
         <is>
           <t>1-</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
         <v>2</v>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Student B, Student F</t>
         </is>

</xml_diff>

<commit_message>
fixed autosave / save / load
</commit_message>
<xml_diff>
--- a/template_sekundarstufe_1.xlsx
+++ b/template_sekundarstufe_1.xlsx
@@ -494,7 +494,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2-</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -502,20 +502,20 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>23.0 (74.2%)</t>
+          <t>22.5 (72.6%)</t>
         </is>
       </c>
       <c r="E2" t="n">
         <v>6</v>
       </c>
       <c r="F2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G2" t="n">
         <v>3</v>
       </c>
       <c r="H2" t="n">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -529,7 +529,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1-</t>
+          <t>2+</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -537,7 +537,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>27.0 (87.1%)</t>
+          <t>25.0 (80.6%)</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -550,7 +550,7 @@
         <v>8</v>
       </c>
       <c r="H3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I3" t="n">
         <v>0</v>
@@ -564,7 +564,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3-</t>
+          <t>2+</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -572,14 +572,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18.0 (58.1%)</t>
+          <t>25.0 (80.6%)</t>
         </is>
       </c>
       <c r="E4" t="n">
         <v>5</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G4" t="n">
         <v>5</v>
@@ -1231,7 +1231,7 @@
     </row>
     <row r="2">
       <c r="A2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
         <v>40</v>
@@ -1334,11 +1334,11 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3-</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -1346,17 +1346,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Student C</t>
+          <t>Student H</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3+</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -1364,17 +1364,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Student H</t>
+          <t>Student I</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>3+</t>
+          <t>2-</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -1382,13 +1382,13 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Student I</t>
+          <t>Student J</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>22</v>
+        <v>22.5</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1400,25 +1400,25 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Student J</t>
+          <t>Student A</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2+</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Student A</t>
+          <t>Student B, Student C</t>
         </is>
       </c>
     </row>
@@ -1432,11 +1432,11 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Student B, Student F</t>
+          <t>Student F</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1479,22 +1479,22 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1-</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Student B, Student F</t>
+          <t>Student F</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2+</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -1502,29 +1502,29 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Student A, Student J</t>
+          <t>Student B, Student C</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2-</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Student C, Student H, Student I</t>
+          <t>Student A, Student J</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -1532,14 +1532,14 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Student G</t>
+          <t>Student H</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3+</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -1547,20 +1547,50 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Student D</t>
+          <t>Student I</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
+          <t>4-</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Student G</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>5-</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Student D</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
           <t>6</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>Student E</t>
         </is>

</xml_diff>